<commit_message>
updated R script, removed rows with failures, script ot make combined bar graph of execution times
</commit_message>
<xml_diff>
--- a/Tilastollinen_Testaus.xlsx
+++ b/Tilastollinen_Testaus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomi\R\gradu_r\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="16">
   <si>
     <t>Tilanne</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>C84:C133</t>
+  </si>
+  <si>
+    <t>T-TEST</t>
+  </si>
+  <si>
+    <t>Appium</t>
+  </si>
+  <si>
+    <t>Espresso</t>
   </si>
 </sst>
 </file>
@@ -428,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,7 +464,7 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -467,7 +476,7 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C15" ca="1" si="0">RANDBETWEEN(10,15)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -476,7 +485,7 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -494,7 +503,7 @@
       </c>
       <c r="C6">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -503,7 +512,7 @@
       </c>
       <c r="C7">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -521,7 +530,7 @@
       </c>
       <c r="C9">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -530,7 +539,7 @@
       </c>
       <c r="C10">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -539,7 +548,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -557,7 +566,7 @@
       </c>
       <c r="C13">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -566,12 +575,12 @@
       </c>
       <c r="C14">
         <f ca="1">RANDBETWEEN(10,15)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
         <v>3</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -590,11 +599,11 @@
       </c>
       <c r="C16">
         <f ca="1">RANDBETWEEN(11,16)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F16">
         <f ca="1">_xlfn.T.TEST(C2:C15,C16:C30,2,2)</f>
-        <v>0.16818344323874598</v>
+        <v>1.3860916693415746E-2</v>
       </c>
       <c r="I16">
         <v>0.05</v>
@@ -606,7 +615,7 @@
       </c>
       <c r="C17">
         <f t="shared" ref="C17:C30" ca="1" si="1">RANDBETWEEN(11,16)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.35">
@@ -615,7 +624,7 @@
       </c>
       <c r="C18">
         <f ca="1">RANDBETWEEN(11,16)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
@@ -624,7 +633,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
@@ -648,11 +657,11 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21">
         <f ca="1">(AVERAGE(C2:C15)-AVERAGE(C16:C30))/(STDEV(C2:C30))</f>
-        <v>-0.51703491456637607</v>
+        <v>-0.88856171353226654</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>2</v>
@@ -664,7 +673,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
@@ -673,7 +682,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
@@ -682,7 +691,7 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.35">
@@ -691,11 +700,11 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H25" s="1">
         <f ca="1">AVERAGE(C16:C30)/AVERAGE(C2:C15)-1</f>
-        <v>6.1538461538461542E-2</v>
+        <v>0.12000000000000011</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
@@ -704,7 +713,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
@@ -713,7 +722,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
@@ -722,7 +731,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.35">
@@ -731,7 +740,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.35">
@@ -740,7 +749,7 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.35">
@@ -752,50 +761,57 @@
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B34">
-        <v>1</v>
+      <c r="B34" t="s">
+        <v>14</v>
       </c>
       <c r="C34">
         <v>520.52</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B35">
-        <v>1</v>
+      <c r="B35" t="s">
+        <v>14</v>
       </c>
       <c r="C35">
         <v>498.61</v>
       </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
       <c r="H35" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B36">
-        <v>1</v>
+      <c r="B36" t="s">
+        <v>14</v>
       </c>
       <c r="C36">
         <v>498.2</v>
       </c>
+      <c r="F36">
+        <f>_xlfn.T.TEST(C34:C83,C84:C133, 2, 2)</f>
+        <v>8.3781313377976937E-130</v>
+      </c>
       <c r="H36">
-        <f>(AVERAGE(C34:C83)-AVERAGE(C84:C133))/(STDEV(C34:C133))</f>
-        <v>1.9875415859959447</v>
+        <f>(AVERAGE(C34:C83)-AVERAGE(C84:C133))/(STDEV(C84:C133))</f>
+        <v>708.97824454250213</v>
       </c>
       <c r="K36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B37">
-        <v>1</v>
+      <c r="B37" t="s">
+        <v>14</v>
       </c>
       <c r="C37">
         <v>500.12</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B38">
-        <v>1</v>
+      <c r="B38" t="s">
+        <v>14</v>
       </c>
       <c r="C38">
         <v>498.6</v>
@@ -805,8 +821,8 @@
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B39">
-        <v>1</v>
+      <c r="B39" t="s">
+        <v>14</v>
       </c>
       <c r="C39">
         <v>497.38</v>
@@ -818,752 +834,752 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B40">
-        <v>1</v>
+      <c r="B40" t="s">
+        <v>14</v>
       </c>
       <c r="C40">
         <v>499.73</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B41">
-        <v>1</v>
+      <c r="B41" t="s">
+        <v>14</v>
       </c>
       <c r="C41">
         <v>499.55</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B42">
-        <v>1</v>
+      <c r="B42" t="s">
+        <v>14</v>
       </c>
       <c r="C42">
         <v>500.31</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B43">
-        <v>1</v>
+      <c r="B43" t="s">
+        <v>14</v>
       </c>
       <c r="C43">
         <v>499.9</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B44">
-        <v>1</v>
+      <c r="B44" t="s">
+        <v>14</v>
       </c>
       <c r="C44">
         <v>499.85</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B45">
-        <v>1</v>
+      <c r="B45" t="s">
+        <v>14</v>
       </c>
       <c r="C45">
         <v>497.97</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B46">
-        <v>1</v>
+      <c r="B46" t="s">
+        <v>14</v>
       </c>
       <c r="C46">
         <v>498.38</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B47">
-        <v>1</v>
+      <c r="B47" t="s">
+        <v>14</v>
       </c>
       <c r="C47">
         <v>500.32</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B48">
-        <v>1</v>
+      <c r="B48" t="s">
+        <v>14</v>
       </c>
       <c r="C48">
         <v>499.39</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49">
-        <v>1</v>
+      <c r="B49" t="s">
+        <v>14</v>
       </c>
       <c r="C49">
         <v>499.63</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50">
-        <v>1</v>
+      <c r="B50" t="s">
+        <v>14</v>
       </c>
       <c r="C50">
         <v>499.88</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51">
-        <v>1</v>
+      <c r="B51" t="s">
+        <v>14</v>
       </c>
       <c r="C51">
         <v>498.82</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52">
-        <v>1</v>
+      <c r="B52" t="s">
+        <v>14</v>
       </c>
       <c r="C52">
         <v>497.93</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53">
-        <v>1</v>
+      <c r="B53" t="s">
+        <v>14</v>
       </c>
       <c r="C53">
         <v>498.02</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54">
-        <v>1</v>
+      <c r="B54" t="s">
+        <v>14</v>
       </c>
       <c r="C54">
         <v>500.43</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55">
-        <v>1</v>
+      <c r="B55" t="s">
+        <v>14</v>
       </c>
       <c r="C55">
         <v>506.15</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56">
-        <v>1</v>
+      <c r="B56" t="s">
+        <v>14</v>
       </c>
       <c r="C56">
         <v>530.12</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57">
-        <v>1</v>
+      <c r="B57" t="s">
+        <v>14</v>
       </c>
       <c r="C57">
         <v>551.54999999999995</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58">
-        <v>1</v>
+      <c r="B58" t="s">
+        <v>14</v>
       </c>
       <c r="C58">
         <v>548.72</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59">
-        <v>1</v>
+      <c r="B59" t="s">
+        <v>14</v>
       </c>
       <c r="C59">
         <v>514.01</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60">
-        <v>1</v>
+      <c r="B60" t="s">
+        <v>14</v>
       </c>
       <c r="C60">
         <v>493.2</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61">
-        <v>1</v>
+      <c r="B61" t="s">
+        <v>14</v>
       </c>
       <c r="C61">
         <v>501.19</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62">
-        <v>1</v>
+      <c r="B62" t="s">
+        <v>14</v>
       </c>
       <c r="C62">
         <v>500.12</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B63">
-        <v>1</v>
+      <c r="B63" t="s">
+        <v>14</v>
       </c>
       <c r="C63">
         <v>500.17</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B64">
-        <v>1</v>
+      <c r="B64" t="s">
+        <v>14</v>
       </c>
       <c r="C64">
         <v>501.4</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B65">
-        <v>1</v>
+      <c r="B65" t="s">
+        <v>14</v>
       </c>
       <c r="C65">
         <v>500</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B66">
-        <v>1</v>
+      <c r="B66" t="s">
+        <v>14</v>
       </c>
       <c r="C66">
         <v>502.2</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B67">
-        <v>1</v>
+      <c r="B67" t="s">
+        <v>14</v>
       </c>
       <c r="C67">
         <v>501.39</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B68">
-        <v>1</v>
+      <c r="B68" t="s">
+        <v>14</v>
       </c>
       <c r="C68">
         <v>502.43</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B69">
-        <v>1</v>
+      <c r="B69" t="s">
+        <v>14</v>
       </c>
       <c r="C69">
         <v>500.35</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70">
-        <v>1</v>
+      <c r="B70" t="s">
+        <v>14</v>
       </c>
       <c r="C70">
         <v>500.41</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B71">
-        <v>1</v>
+      <c r="B71" t="s">
+        <v>14</v>
       </c>
       <c r="C71">
         <v>518.35</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B72">
-        <v>1</v>
+      <c r="B72" t="s">
+        <v>14</v>
       </c>
       <c r="C72">
         <v>545.41</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B73">
-        <v>1</v>
+      <c r="B73" t="s">
+        <v>14</v>
       </c>
       <c r="C73">
         <v>552.97</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74">
-        <v>1</v>
+      <c r="B74" t="s">
+        <v>14</v>
       </c>
       <c r="C74">
         <v>535.16</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B75">
-        <v>1</v>
+      <c r="B75" t="s">
+        <v>14</v>
       </c>
       <c r="C75">
         <v>503.34</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B76">
-        <v>1</v>
+      <c r="B76" t="s">
+        <v>14</v>
       </c>
       <c r="C76">
         <v>503.54</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B77">
-        <v>1</v>
+      <c r="B77" t="s">
+        <v>14</v>
       </c>
       <c r="C77">
         <v>502.43</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B78">
-        <v>1</v>
+      <c r="B78" t="s">
+        <v>14</v>
       </c>
       <c r="C78">
         <v>498.49</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B79">
-        <v>1</v>
+      <c r="B79" t="s">
+        <v>14</v>
       </c>
       <c r="C79">
         <v>496.35</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B80">
-        <v>1</v>
+      <c r="B80" t="s">
+        <v>14</v>
       </c>
       <c r="C80">
         <v>500.32</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81">
-        <v>1</v>
+      <c r="B81" t="s">
+        <v>14</v>
       </c>
       <c r="C81">
         <v>501.89</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B82">
-        <v>1</v>
+      <c r="B82" t="s">
+        <v>14</v>
       </c>
       <c r="C82">
         <v>500.91</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B83">
-        <v>1</v>
+      <c r="B83" t="s">
+        <v>14</v>
       </c>
       <c r="C83">
         <v>500.01</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B84">
-        <v>2</v>
+      <c r="B84" t="s">
+        <v>15</v>
       </c>
       <c r="C84">
         <v>79.37</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B85">
-        <v>2</v>
+      <c r="B85" t="s">
+        <v>15</v>
       </c>
       <c r="C85">
         <v>79.510000000000005</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B86">
-        <v>2</v>
+      <c r="B86" t="s">
+        <v>15</v>
       </c>
       <c r="C86">
         <v>78.349999999999994</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B87">
-        <v>2</v>
+      <c r="B87" t="s">
+        <v>15</v>
       </c>
       <c r="C87">
         <v>78.69</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B88">
-        <v>2</v>
+      <c r="B88" t="s">
+        <v>15</v>
       </c>
       <c r="C88">
         <v>79.47</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B89">
-        <v>2</v>
+      <c r="B89" t="s">
+        <v>15</v>
       </c>
       <c r="C89">
         <v>78.5</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B90">
-        <v>2</v>
+      <c r="B90" t="s">
+        <v>15</v>
       </c>
       <c r="C90">
         <v>78.2</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B91">
-        <v>2</v>
+      <c r="B91" t="s">
+        <v>15</v>
       </c>
       <c r="C91">
         <v>78.64</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B92">
-        <v>2</v>
+      <c r="B92" t="s">
+        <v>15</v>
       </c>
       <c r="C92">
         <v>78.78</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B93">
-        <v>2</v>
+      <c r="B93" t="s">
+        <v>15</v>
       </c>
       <c r="C93">
         <v>79.36</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94">
-        <v>2</v>
+      <c r="B94" t="s">
+        <v>15</v>
       </c>
       <c r="C94">
         <v>78.37</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95">
-        <v>2</v>
+      <c r="B95" t="s">
+        <v>15</v>
       </c>
       <c r="C95">
         <v>78.36</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B96">
-        <v>2</v>
+      <c r="B96" t="s">
+        <v>15</v>
       </c>
       <c r="C96">
         <v>78.430000000000007</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97">
-        <v>2</v>
+      <c r="B97" t="s">
+        <v>15</v>
       </c>
       <c r="C97">
         <v>78.33</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B98">
-        <v>2</v>
+      <c r="B98" t="s">
+        <v>15</v>
       </c>
       <c r="C98">
         <v>79.239999999999995</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B99">
-        <v>2</v>
+      <c r="B99" t="s">
+        <v>15</v>
       </c>
       <c r="C99">
         <v>79.36</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B100">
-        <v>2</v>
+      <c r="B100" t="s">
+        <v>15</v>
       </c>
       <c r="C100">
         <v>78.63</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B101">
-        <v>2</v>
+      <c r="B101" t="s">
+        <v>15</v>
       </c>
       <c r="C101">
         <v>78.28</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B102">
-        <v>2</v>
+      <c r="B102" t="s">
+        <v>15</v>
       </c>
       <c r="C102">
         <v>78.069999999999993</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B103">
-        <v>2</v>
+      <c r="B103" t="s">
+        <v>15</v>
       </c>
       <c r="C103">
         <v>79.78</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B104">
-        <v>2</v>
+      <c r="B104" t="s">
+        <v>15</v>
       </c>
       <c r="C104">
         <v>78.84</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B105">
-        <v>2</v>
+      <c r="B105" t="s">
+        <v>15</v>
       </c>
       <c r="C105">
         <v>78.760000000000005</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B106">
-        <v>2</v>
+      <c r="B106" t="s">
+        <v>15</v>
       </c>
       <c r="C106">
         <v>78.989999999999995</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B107">
-        <v>2</v>
+      <c r="B107" t="s">
+        <v>15</v>
       </c>
       <c r="C107">
         <v>78.95</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B108">
-        <v>2</v>
+      <c r="B108" t="s">
+        <v>15</v>
       </c>
       <c r="C108">
         <v>78.33</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B109">
-        <v>2</v>
+      <c r="B109" t="s">
+        <v>15</v>
       </c>
       <c r="C109">
         <v>78.55</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B110">
-        <v>2</v>
+      <c r="B110" t="s">
+        <v>15</v>
       </c>
       <c r="C110">
         <v>78.64</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B111">
-        <v>2</v>
+      <c r="B111" t="s">
+        <v>15</v>
       </c>
       <c r="C111">
         <v>78.67</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B112">
-        <v>2</v>
+      <c r="B112" t="s">
+        <v>15</v>
       </c>
       <c r="C112">
         <v>78.599999999999994</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B113">
-        <v>2</v>
+      <c r="B113" t="s">
+        <v>15</v>
       </c>
       <c r="C113">
         <v>78.650000000000006</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B114">
-        <v>2</v>
+      <c r="B114" t="s">
+        <v>15</v>
       </c>
       <c r="C114">
         <v>78.72</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B115">
-        <v>2</v>
+      <c r="B115" t="s">
+        <v>15</v>
       </c>
       <c r="C115">
         <v>78.33</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B116">
-        <v>2</v>
+      <c r="B116" t="s">
+        <v>15</v>
       </c>
       <c r="C116">
         <v>78.28</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B117">
-        <v>2</v>
+      <c r="B117" t="s">
+        <v>15</v>
       </c>
       <c r="C117">
         <v>79.31</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B118">
-        <v>2</v>
+      <c r="B118" t="s">
+        <v>15</v>
       </c>
       <c r="C118">
         <v>78.2</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B119">
-        <v>2</v>
+      <c r="B119" t="s">
+        <v>15</v>
       </c>
       <c r="C119">
         <v>78.61</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B120">
-        <v>2</v>
+      <c r="B120" t="s">
+        <v>15</v>
       </c>
       <c r="C120">
         <v>78.64</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B121">
-        <v>2</v>
+      <c r="B121" t="s">
+        <v>15</v>
       </c>
       <c r="C121">
         <v>78.63</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B122">
-        <v>2</v>
+      <c r="B122" t="s">
+        <v>15</v>
       </c>
       <c r="C122">
         <v>78.44</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B123">
-        <v>2</v>
+      <c r="B123" t="s">
+        <v>15</v>
       </c>
       <c r="C123">
         <v>77.92</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B124">
-        <v>2</v>
+      <c r="B124" t="s">
+        <v>15</v>
       </c>
       <c r="C124">
         <v>78.709999999999994</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B125">
-        <v>2</v>
+      <c r="B125" t="s">
+        <v>15</v>
       </c>
       <c r="C125">
         <v>78.41</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B126">
-        <v>2</v>
+      <c r="B126" t="s">
+        <v>15</v>
       </c>
       <c r="C126">
         <v>81.180000000000007</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B127">
-        <v>2</v>
+      <c r="B127" t="s">
+        <v>15</v>
       </c>
       <c r="C127">
         <v>80.3</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B128">
-        <v>2</v>
+      <c r="B128" t="s">
+        <v>15</v>
       </c>
       <c r="C128">
         <v>78.55</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B129">
-        <v>2</v>
+      <c r="B129" t="s">
+        <v>15</v>
       </c>
       <c r="C129">
         <v>78.13</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B130">
-        <v>2</v>
+      <c r="B130" t="s">
+        <v>15</v>
       </c>
       <c r="C130">
         <v>78.83</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B131">
-        <v>2</v>
+      <c r="B131" t="s">
+        <v>15</v>
       </c>
       <c r="C131">
         <v>79.5</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B132">
-        <v>2</v>
+      <c r="B132" t="s">
+        <v>15</v>
       </c>
       <c r="C132">
         <v>78.709999999999994</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B133">
-        <v>2</v>
+      <c r="B133" t="s">
+        <v>15</v>
       </c>
       <c r="C133">
         <v>77.83</v>
@@ -1572,8 +1588,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J21" r:id="rId1" location="Cohen.27s_d"/>
+    <hyperlink ref="G14" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>